<commit_message>
Refatorações e correção de bugs
</commit_message>
<xml_diff>
--- a/massa de dados/Massa.xlsx
+++ b/massa de dados/Massa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.cardoso\workspace\AppiumTDD\massa de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679D46A0-2598-440F-809A-FEBD05B2C1F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18909FB-1292-4519-A465-68C04DB88A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1515" windowWidth="11070" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
     <t>55999911011</t>
   </si>
   <si>
-    <t>JurlinFrefas03</t>
+    <t>TesteTeste16</t>
   </si>
 </sst>
 </file>

</xml_diff>